<commit_message>
getting ready to changing the verbose output to be less cluttered
</commit_message>
<xml_diff>
--- a/processed_data/nikon_cellpose_bags_spots_results.xlsx
+++ b/processed_data/nikon_cellpose_bags_spots_results.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -731,22 +731,22 @@
         <v>1</v>
       </c>
       <c r="B9" t="n">
-        <v>425</v>
+        <v>120</v>
       </c>
       <c r="C9" t="n">
-        <v>483620</v>
+        <v>535894</v>
       </c>
       <c r="D9" t="n">
-        <v>25196.69159081848</v>
+        <v>27920.17667460005</v>
       </c>
       <c r="E9" t="n">
-        <v>503933.8318163696</v>
+        <v>558403.5334920011</v>
       </c>
       <c r="F9" t="n">
-        <v>0.01686729380594028</v>
+        <v>0.004297967072291778</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0008433646902970139</v>
+        <v>0.0002148983536145889</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -755,11 +755,11 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>lig1ON_P</t>
+          <t>P_None_No</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -767,22 +767,22 @@
         <v>2</v>
       </c>
       <c r="B10" t="n">
-        <v>454</v>
+        <v>101</v>
       </c>
       <c r="C10" t="n">
-        <v>499680</v>
+        <v>482984</v>
       </c>
       <c r="D10" t="n">
-        <v>26033.42056594057</v>
+        <v>25163.5558729992</v>
       </c>
       <c r="E10" t="n">
-        <v>520668.4113188114</v>
+        <v>503271.1174599839</v>
       </c>
       <c r="F10" t="n">
-        <v>0.01743912210268544</v>
+        <v>0.004013741162407584</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0008719561051342723</v>
+        <v>0.0002006870581203792</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -791,11 +791,11 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>lig1ON_P</t>
+          <t>P_None_No</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
@@ -803,22 +803,22 @@
         <v>2</v>
       </c>
       <c r="B11" t="n">
-        <v>413</v>
+        <v>114</v>
       </c>
       <c r="C11" t="n">
-        <v>408840</v>
+        <v>565643</v>
       </c>
       <c r="D11" t="n">
-        <v>21300.63973779047</v>
+        <v>29470.10508561544</v>
       </c>
       <c r="E11" t="n">
-        <v>426012.7947558094</v>
+        <v>589402.1017123087</v>
       </c>
       <c r="F11" t="n">
-        <v>0.01938908901723159</v>
+        <v>0.003868326891567285</v>
       </c>
       <c r="G11" t="n">
-        <v>0.0009694544508615796</v>
+        <v>0.0001934163445783643</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
@@ -827,11 +827,11 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>lig1ON_P</t>
+          <t>P_None_No</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12">
@@ -839,22 +839,22 @@
         <v>1</v>
       </c>
       <c r="B12" t="n">
-        <v>439</v>
+        <v>91</v>
       </c>
       <c r="C12" t="n">
-        <v>450060</v>
+        <v>267342</v>
       </c>
       <c r="D12" t="n">
-        <v>23448.20937381366</v>
+        <v>13928.56772522351</v>
       </c>
       <c r="E12" t="n">
-        <v>468964.1874762733</v>
+        <v>278571.3545044702</v>
       </c>
       <c r="F12" t="n">
-        <v>0.01872211191061197</v>
+        <v>0.006533335070425537</v>
       </c>
       <c r="G12" t="n">
-        <v>0.0009361055955305984</v>
+        <v>0.0003266667535212769</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
@@ -863,11 +863,11 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>lig1ON_P</t>
+          <t>P_None_No</t>
         </is>
       </c>
       <c r="J12" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
@@ -875,22 +875,22 @@
         <v>2</v>
       </c>
       <c r="B13" t="n">
-        <v>460</v>
+        <v>108</v>
       </c>
       <c r="C13" t="n">
-        <v>473030</v>
+        <v>281652</v>
       </c>
       <c r="D13" t="n">
-        <v>24644.9506290163</v>
+        <v>14674.12137615733</v>
       </c>
       <c r="E13" t="n">
-        <v>492899.0125803261</v>
+        <v>293482.4275231465</v>
       </c>
       <c r="F13" t="n">
-        <v>0.01866508101089106</v>
+        <v>0.007359895507984525</v>
       </c>
       <c r="G13" t="n">
-        <v>0.0009332540505445532</v>
+        <v>0.0003679947753992263</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
@@ -899,34 +899,34 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>lig1ON_P</t>
+          <t>P_None_No</t>
         </is>
       </c>
       <c r="J13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B14" t="n">
-        <v>447</v>
+        <v>122</v>
       </c>
       <c r="C14" t="n">
-        <v>521040</v>
+        <v>269392</v>
       </c>
       <c r="D14" t="n">
-        <v>27146.28052289</v>
+        <v>14035.37310498691</v>
       </c>
       <c r="E14" t="n">
-        <v>542925.6104577999</v>
+        <v>280707.4620997383</v>
       </c>
       <c r="F14" t="n">
-        <v>0.01646634424274388</v>
+        <v>0.008692323252643146</v>
       </c>
       <c r="G14" t="n">
-        <v>0.000823317212137194</v>
+        <v>0.0004346161626321573</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -935,7 +935,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>lig1ON_P</t>
+          <t>P_None_No</t>
         </is>
       </c>
       <c r="J14" t="n">
@@ -944,25 +944,25 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B15" t="n">
-        <v>462</v>
+        <v>114</v>
       </c>
       <c r="C15" t="n">
-        <v>502940</v>
+        <v>416163</v>
       </c>
       <c r="D15" t="n">
-        <v>26203.26716985701</v>
+        <v>21682.16939437945</v>
       </c>
       <c r="E15" t="n">
-        <v>524065.3433971402</v>
+        <v>433643.3878875891</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0176313891319424</v>
+        <v>0.005257776467217879</v>
       </c>
       <c r="G15" t="n">
-        <v>0.0008815694565971202</v>
+        <v>0.0002628888233608939</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -971,34 +971,34 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>lig1ON_P</t>
+          <t>P_None_No</t>
         </is>
       </c>
       <c r="J15" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B16" t="n">
-        <v>471</v>
+        <v>115</v>
       </c>
       <c r="C16" t="n">
-        <v>538150</v>
+        <v>481085</v>
       </c>
       <c r="D16" t="n">
-        <v>28037.71469252505</v>
+        <v>25064.61762120861</v>
       </c>
       <c r="E16" t="n">
-        <v>560754.293850501</v>
+        <v>501292.3524241722</v>
       </c>
       <c r="F16" t="n">
-        <v>0.01679880137041163</v>
+        <v>0.004588141009687373</v>
       </c>
       <c r="G16" t="n">
-        <v>0.0008399400685205814</v>
+        <v>0.0002294070504843687</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -1007,47 +1007,299 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>lig1ON_P</t>
+          <t>P_None_No</t>
         </is>
       </c>
       <c r="J16" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
+        <v>4</v>
+      </c>
+      <c r="B17" t="n">
+        <v>123</v>
+      </c>
+      <c r="C17" t="n">
+        <v>454033</v>
+      </c>
+      <c r="D17" t="n">
+        <v>23655.20340981367</v>
+      </c>
+      <c r="E17" t="n">
+        <v>473104.0681962734</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.005199701641498963</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.0002599850820749481</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>nikon_cellpose_bags_spots</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>P_None_No</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>5</v>
+      </c>
+      <c r="B18" t="n">
+        <v>130</v>
+      </c>
+      <c r="C18" t="n">
+        <v>439263</v>
+      </c>
+      <c r="D18" t="n">
+        <v>22885.68367366465</v>
+      </c>
+      <c r="E18" t="n">
+        <v>457713.673473293</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.005680407098766095</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.0002840203549383048</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>nikon_cellpose_bags_spots</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>P_None_No</t>
+        </is>
+      </c>
+      <c r="J18" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
         <v>1</v>
       </c>
-      <c r="B17" t="n">
-        <v>497</v>
-      </c>
-      <c r="C17" t="n">
-        <v>502370</v>
-      </c>
-      <c r="D17" t="n">
-        <v>26173.57006426426</v>
-      </c>
-      <c r="E17" t="n">
-        <v>523471.4012852851</v>
-      </c>
-      <c r="F17" t="n">
-        <v>0.01898862091719664</v>
-      </c>
-      <c r="G17" t="n">
-        <v>0.0009494310458598319</v>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>nikon_cellpose_bags_spots</t>
-        </is>
-      </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>lig1ON_P</t>
-        </is>
-      </c>
-      <c r="J17" t="n">
+      <c r="B19" t="n">
+        <v>122</v>
+      </c>
+      <c r="C19" t="n">
+        <v>750346</v>
+      </c>
+      <c r="D19" t="n">
+        <v>39093.16560192771</v>
+      </c>
+      <c r="E19" t="n">
+        <v>781863.3120385543</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.003120750088194037</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.0001560375044097018</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>nikon_cellpose_bags_spots</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>P_None_No</t>
+        </is>
+      </c>
+      <c r="J19" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>2</v>
+      </c>
+      <c r="B20" t="n">
+        <v>131</v>
+      </c>
+      <c r="C20" t="n">
+        <v>717257</v>
+      </c>
+      <c r="D20" t="n">
+        <v>37369.22257217586</v>
+      </c>
+      <c r="E20" t="n">
+        <v>747384.4514435171</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.003505558611688624</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.0001752779305844312</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>nikon_cellpose_bags_spots</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>P_None_No</t>
+        </is>
+      </c>
+      <c r="J20" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>1</v>
+      </c>
+      <c r="B21" t="n">
+        <v>121</v>
+      </c>
+      <c r="C21" t="n">
+        <v>375962</v>
+      </c>
+      <c r="D21" t="n">
+        <v>19587.68984712646</v>
+      </c>
+      <c r="E21" t="n">
+        <v>391753.7969425292</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.006177349189432407</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0.0003088674594716203</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>nikon_cellpose_bags_spots</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>P_None_No</t>
+        </is>
+      </c>
+      <c r="J21" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>2</v>
+      </c>
+      <c r="B22" t="n">
+        <v>107</v>
+      </c>
+      <c r="C22" t="n">
+        <v>348514</v>
+      </c>
+      <c r="D22" t="n">
+        <v>18157.64396237234</v>
+      </c>
+      <c r="E22" t="n">
+        <v>363152.8792474468</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.005892835007764971</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0.0002946417503882486</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>nikon_cellpose_bags_spots</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>P_None_No</t>
+        </is>
+      </c>
+      <c r="J22" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>1</v>
+      </c>
+      <c r="B23" t="n">
+        <v>7</v>
+      </c>
+      <c r="C23" t="n">
+        <v>286682</v>
+      </c>
+      <c r="D23" t="n">
+        <v>14936.18530796705</v>
+      </c>
+      <c r="E23" t="n">
+        <v>298723.7061593409</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.0004686604950104736</v>
+      </c>
+      <c r="G23" t="n">
+        <v>2.343302475052368e-05</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>nikon_cellpose_bags_spots</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>None_0</t>
+        </is>
+      </c>
+      <c r="J23" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>1</v>
+      </c>
+      <c r="B24" t="n">
         <v>6</v>
+      </c>
+      <c r="C24" t="n">
+        <v>944338</v>
+      </c>
+      <c r="D24" t="n">
+        <v>49200.18473903135</v>
+      </c>
+      <c r="E24" t="n">
+        <v>984003.694780627</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.0001219507616043583</v>
+      </c>
+      <c r="G24" t="n">
+        <v>6.097538080217915e-06</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>nikon_cellpose_bags_spots</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>None_0</t>
+        </is>
+      </c>
+      <c r="J24" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1061,7 +1313,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1129,35 +1381,35 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>allON_HP</t>
+          <t>None_0</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>650.429</v>
+        <v>6.5</v>
       </c>
       <c r="D2" t="n">
-        <v>115.299</v>
+        <v>0.707</v>
       </c>
       <c r="E2" t="n">
-        <v>4553</v>
+        <v>13</v>
       </c>
       <c r="F2" t="n">
-        <v>22036.741</v>
+        <v>32068.185</v>
       </c>
       <c r="G2" t="n">
-        <v>5712.431</v>
+        <v>24228.306</v>
       </c>
       <c r="H2" t="n">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>0.003</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
@@ -1166,37 +1418,74 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>lig1ON_P</t>
+          <t>P_None_No</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C3" t="n">
-        <v>452</v>
+        <v>115.643</v>
       </c>
       <c r="D3" t="n">
-        <v>24.995</v>
+        <v>11.043</v>
       </c>
       <c r="E3" t="n">
-        <v>4068</v>
+        <v>1619</v>
       </c>
       <c r="F3" t="n">
-        <v>25353.86</v>
+        <v>23763.378</v>
       </c>
       <c r="G3" t="n">
-        <v>2026.648</v>
+        <v>7852.325</v>
       </c>
       <c r="H3" t="n">
-        <v>0.018</v>
+        <v>0.005</v>
       </c>
       <c r="I3" t="n">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="J3" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>allON_HP</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>7</v>
+      </c>
+      <c r="C4" t="n">
+        <v>650.429</v>
+      </c>
+      <c r="D4" t="n">
+        <v>115.299</v>
+      </c>
+      <c r="E4" t="n">
+        <v>4553</v>
+      </c>
+      <c r="F4" t="n">
+        <v>22036.741</v>
+      </c>
+      <c r="G4" t="n">
+        <v>5712.431</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="K4" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>